<commit_message>
Added the config for mobile dev (evening)
</commit_message>
<xml_diff>
--- a/backend-frameworks-zc0014/config.xlsx
+++ b/backend-frameworks-zc0014/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\canvas-course-scaffolder-with-course-configs\backend-frameworks-zc0014\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986BB8F5-EC9E-4C10-8B74-3B68B6FC237E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D5EF81-F507-4F23-8D23-C16FCBBACEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="27708" windowHeight="16560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemene info" sheetId="1" r:id="rId1"/>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1181C0AF-0EEA-45EA-A4B8-73E6C5261177}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1011,13 +1011,13 @@
         <v>37</v>
       </c>
       <c r="C2" s="1">
-        <v>45030.999305555553</v>
+        <v>45396.999305555553</v>
       </c>
       <c r="D2" s="1">
         <v>45243.354166666664</v>
       </c>
       <c r="E2" s="1">
-        <v>45030.999305555553</v>
+        <v>45396.999305555553</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1296,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E63DFD8-2013-40A2-8CE5-0CB5ABE5CD54}">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>

</xml_diff>